<commit_message>
Updated Supply Chain twins
</commit_message>
<xml_diff>
--- a/sandbox/AzureDigitalTwins/logistics-supply-chain-twin.xlsx
+++ b/sandbox/AzureDigitalTwins/logistics-supply-chain-twin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\vscode\industryx-sandbox\industryx\sandbox\AzureDigitalTwins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC75240-814D-460F-ADBB-990551A13705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0726DA22-885F-459A-8E61-3335F60DB982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3308" yWindow="1230" windowWidth="18667" windowHeight="20670" xr2:uid="{B6154E4F-774F-4730-84F3-5195ADBCD94E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="30">
   <si>
     <t>ModelID</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>RETAIL-STORE-3</t>
+  </si>
+  <si>
+    <t>RETAIL-STORE-4</t>
   </si>
 </sst>
 </file>
@@ -480,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E4B3A2-EF53-41B2-9F0F-6F5502ACE162}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -771,6 +774,20 @@
         <v>26</v>
       </c>
     </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E21" xr:uid="{5093E85F-94E4-4979-9E01-3F5F25EDF789}"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>